<commit_message>
gestion fichiers texte + excel
</commit_message>
<xml_diff>
--- a/resources/inputDataExcel.xlsx
+++ b/resources/inputDataExcel.xlsx
@@ -5,132 +5,81 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo t490\eclipse-workspace\JoueurProjet\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE58219-42F8-45A4-B5CA-E6430A1A949C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6790340-65DC-4BBA-A0A4-F243B2E03F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name=" Liste des joueurs " sheetId="1" r:id="rId1"/>
+    <sheet name="Joueurs" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
-  <si>
-    <t>IDJoueur</t>
-  </si>
-  <si>
-    <t>NomJoueur</t>
-  </si>
-  <si>
-    <t>PrenomJoueur</t>
-  </si>
-  <si>
-    <t>salaire</t>
-  </si>
-  <si>
-    <t>numero</t>
-  </si>
-  <si>
-    <t>matchs</t>
-  </si>
-  <si>
-    <t>buts</t>
-  </si>
-  <si>
-    <t>poste</t>
-  </si>
-  <si>
-    <t>club</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Messi</t>
-  </si>
-  <si>
-    <t>Lionel</t>
-  </si>
-  <si>
-    <t>50000</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>70</t>
-  </si>
-  <si>
-    <t>Attaquant</t>
-  </si>
-  <si>
-    <t>Barcelona</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Ronaldo</t>
-  </si>
-  <si>
-    <t>Cristiano</t>
-  </si>
-  <si>
-    <t>60000</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>400</t>
-  </si>
-  <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>RealMadrid</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Nakkach</t>
-  </si>
-  <si>
-    <t>Ibrahim</t>
-  </si>
-  <si>
-    <t>20000</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>900</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>Milieu</t>
-  </si>
-  <si>
-    <t>Wydad</t>
-  </si>
-  <si>
-    <t>dateNaissance</t>
-  </si>
-  <si>
-    <t>11/01/1990</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>Prénom</t>
+  </si>
+  <si>
+    <t>Salaire</t>
+  </si>
+  <si>
+    <t>Numéro</t>
+  </si>
+  <si>
+    <t>Matchs</t>
+  </si>
+  <si>
+    <t>Buts</t>
+  </si>
+  <si>
+    <t>Poste</t>
+  </si>
+  <si>
+    <t>Equipe</t>
+  </si>
+  <si>
+    <t>Date de naissance</t>
+  </si>
+  <si>
+    <t>DD</t>
+  </si>
+  <si>
+    <t>DDOO</t>
+  </si>
+  <si>
+    <t>BARCALONA FC</t>
+  </si>
+  <si>
+    <t>11/12/2001</t>
+  </si>
+  <si>
+    <t>TT</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>YYY</t>
+  </si>
+  <si>
+    <t>FF</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>RRR</t>
+  </si>
+  <si>
+    <t>GGG</t>
   </si>
 </sst>
 </file>
@@ -482,15 +431,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -518,104 +467,118 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>35</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>1200</v>
+      </c>
+      <c r="F2">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>1290</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="H2" t="s">
+      <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="I2" t="s">
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>290</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
         <v>17</v>
       </c>
-      <c r="J2" t="s">
-        <v>36</v>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J4" t="s">
-        <v>36</v>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>290</v>
+      </c>
+      <c r="F5">
+        <v>8</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>